<commit_message>
attempt to add TOC filtering - not working
</commit_message>
<xml_diff>
--- a/2_Route_and_times_metadata/route_and_time_metadata.xlsx
+++ b/2_Route_and_times_metadata/route_and_time_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\2_Route_and_times_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>Route6 - All TOCS</t>
+  </si>
+  <si>
+    <t>TOC_Filter</t>
+  </si>
+  <si>
+    <t>All TOCs</t>
   </si>
 </sst>
 </file>
@@ -500,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,86 +546,85 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="1"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>36</v>
+      <c r="D5" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>44</v>
@@ -634,16 +639,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>44</v>
@@ -658,72 +663,96 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>39</v>
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revert "Revert "Updated supporting files""
This reverts commit 91b4fb835362fdf44650f5f226479b0d66ee48b1.
</commit_message>
<xml_diff>
--- a/2_Route_and_times_metadata/route_and_time_metadata.xlsx
+++ b/2_Route_and_times_metadata/route_and_time_metadata.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -60,24 +60,114 @@
     <t>KGX,DON</t>
   </si>
   <si>
+    <t>GRA,KGX</t>
+  </si>
+  <si>
+    <t>CHD,STP</t>
+  </si>
+  <si>
+    <t>LEI,STP</t>
+  </si>
+  <si>
+    <t>YRK,KGX</t>
+  </si>
+  <si>
+    <t>LDS,KGX</t>
+  </si>
+  <si>
     <t>0714,0717,0747,0831</t>
   </si>
   <si>
+    <t>0726,0801,0818</t>
+  </si>
+  <si>
+    <t>0701,0737,0742</t>
+  </si>
+  <si>
+    <t>0707,0755</t>
+  </si>
+  <si>
+    <t>0700,0740</t>
+  </si>
+  <si>
     <t>1425,1430</t>
   </si>
   <si>
+    <t>1418,1501</t>
+  </si>
+  <si>
     <t>1437,1528</t>
   </si>
   <si>
+    <t>1418,1412</t>
+  </si>
+  <si>
+    <t>1501</t>
+  </si>
+  <si>
+    <t>1417</t>
+  </si>
+  <si>
+    <t>1400,1552</t>
+  </si>
+  <si>
+    <t>1405</t>
+  </si>
+  <si>
+    <t>KGX,GRA</t>
+  </si>
+  <si>
+    <t>STP,CHD</t>
+  </si>
+  <si>
+    <t>STP,LEI</t>
+  </si>
+  <si>
+    <t>KGX,YRK</t>
+  </si>
+  <si>
+    <t>1631,1702</t>
+  </si>
+  <si>
     <t>1048,1103,1147</t>
   </si>
   <si>
+    <t>1102</t>
+  </si>
+  <si>
     <t>1448,1448,1550</t>
   </si>
   <si>
+    <t>1432</t>
+  </si>
+  <si>
+    <t>1413</t>
+  </si>
+  <si>
+    <t>1403</t>
+  </si>
+  <si>
+    <t>1351,1357</t>
+  </si>
+  <si>
+    <t>1415</t>
+  </si>
+  <si>
+    <t>KGX,LDS</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
     <t>Route 1 - All TOCS</t>
   </si>
   <si>
+    <t>Route2 - All TOCS</t>
+  </si>
+  <si>
+    <t>Route3 - All TOCS</t>
+  </si>
+  <si>
     <t>1627,1630,1703</t>
   </si>
   <si>
@@ -85,6 +175,123 @@
   </si>
   <si>
     <t>All TOCs</t>
+  </si>
+  <si>
+    <t>Route 1 - GC</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>Route 1 - GR</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>Route 1- HT</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>0831</t>
+  </si>
+  <si>
+    <t>1627</t>
+  </si>
+  <si>
+    <t>1048</t>
+  </si>
+  <si>
+    <t>1550</t>
+  </si>
+  <si>
+    <t>0717</t>
+  </si>
+  <si>
+    <t>1425</t>
+  </si>
+  <si>
+    <t>1528</t>
+  </si>
+  <si>
+    <t>1147</t>
+  </si>
+  <si>
+    <t>1448</t>
+  </si>
+  <si>
+    <t>0714,0747</t>
+  </si>
+  <si>
+    <t>1430</t>
+  </si>
+  <si>
+    <t>1437</t>
+  </si>
+  <si>
+    <t>1630,1703</t>
+  </si>
+  <si>
+    <t>1103</t>
+  </si>
+  <si>
+    <t>Route2 - HT</t>
+  </si>
+  <si>
+    <t>0801</t>
+  </si>
+  <si>
+    <t>1418</t>
+  </si>
+  <si>
+    <t>Route2 - GR</t>
+  </si>
+  <si>
+    <t>0726,0818</t>
+  </si>
+  <si>
+    <t>1412</t>
+  </si>
+  <si>
+    <t>0701,0802,0821</t>
+  </si>
+  <si>
+    <t>Route3 - GC</t>
+  </si>
+  <si>
+    <t>0821</t>
+  </si>
+  <si>
+    <t>1351</t>
+  </si>
+  <si>
+    <t>1552</t>
+  </si>
+  <si>
+    <t>Route3 - GR</t>
+  </si>
+  <si>
+    <t>0701,0802</t>
+  </si>
+  <si>
+    <t>1357</t>
+  </si>
+  <si>
+    <t>1400</t>
+  </si>
+  <si>
+    <t>Route4 - EM</t>
+  </si>
+  <si>
+    <t>EM</t>
+  </si>
+  <si>
+    <t>Route5 - EM</t>
+  </si>
+  <si>
+    <t>Route6 - GR</t>
   </si>
 </sst>
 </file>
@@ -120,9 +327,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,102 +613,464 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="4" width="18.7109375" style="3" customWidth="1"/>
+    <col min="5" max="15" width="18.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>44</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" t="s">
+        <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>49</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" t="s">
+        <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>34</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P6" s="1"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P7" s="1"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>16</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="1"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P9" s="1"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code amended to remove old package and to amend exported data files
Now has all, fixed and relative datafile exports.  Most in combine_data.py
</commit_message>
<xml_diff>
--- a/2_Route_and_times_metadata/route_and_time_metadata.xlsx
+++ b/2_Route_and_times_metadata/route_and_time_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\2_Route_and_times_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\RME_Rail_Fares\2_Route_and_times_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="92">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -292,6 +292,15 @@
   </si>
   <si>
     <t>Route6 - GR</t>
+  </si>
+  <si>
+    <t>Project Type</t>
+  </si>
+  <si>
+    <t>departing on 11/09/2019</t>
+  </si>
+  <si>
+    <t>1,7,30 days ahead from today</t>
   </si>
 </sst>
 </file>
@@ -327,12 +336,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -613,22 +623,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
-    <col min="3" max="4" width="18.7109375" style="3" customWidth="1"/>
-    <col min="5" max="15" width="18.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -672,7 +680,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -716,360 +724,399 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L5" s="2" t="s">
+      <c r="F6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="M6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="M7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="M8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1081,14 +1128,466 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
xlsxl added to gitignore
</commit_message>
<xml_diff>
--- a/2_Route_and_times_metadata/route_and_time_metadata.xlsx
+++ b/2_Route_and_times_metadata/route_and_time_metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\RME_Rail_Fares\2_Route_and_times_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gwilliams\Documents\GitHub\RME_Rail_Fares\2_Route_and_times_metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="93">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -301,6 +301,9 @@
   </si>
   <si>
     <t>1,7,30 days ahead from today</t>
+  </si>
+  <si>
+    <t>departing on 29/02/2020</t>
   </si>
 </sst>
 </file>
@@ -626,7 +629,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,7 +735,7 @@
         <v>91</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>91</v>
@@ -740,23 +743,23 @@
       <c r="E3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>90</v>
+      <c r="F3" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>90</v>
+      <c r="H3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>91</v>
@@ -764,8 +767,8 @@
       <c r="M3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>90</v>
+      <c r="N3" s="5" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Debugging - inconsistent behaviour of upand down routes
print statements added to expose up and downlists
</commit_message>
<xml_diff>
--- a/2_Route_and_times_metadata/route_and_time_metadata.xlsx
+++ b/2_Route_and_times_metadata/route_and_time_metadata.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="92">
   <si>
     <t>origin and destination down</t>
   </si>
@@ -301,9 +301,6 @@
   </si>
   <si>
     <t>1,7,30 days ahead from today</t>
-  </si>
-  <si>
-    <t>departing on 29/02/2020</t>
   </si>
 </sst>
 </file>
@@ -626,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="N11" sqref="C1:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,489 +636,104 @@
     <col min="3" max="3" width="18.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" t="s">
-        <v>77</v>
-      </c>
-      <c r="K1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L1" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" t="s">
-        <v>87</v>
-      </c>
-      <c r="N1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" t="s">
-        <v>49</v>
-      </c>
-      <c r="J2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" t="s">
-        <v>53</v>
-      </c>
-      <c r="L2" t="s">
-        <v>86</v>
-      </c>
-      <c r="M2" t="s">
-        <v>86</v>
-      </c>
-      <c r="N2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C7"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C8"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C9"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C10"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="C11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>